<commit_message>
copied some cells from template xlsx to invoice xlsx
</commit_message>
<xml_diff>
--- a/input_files/invoice_template.xlsx
+++ b/input_files/invoice_template.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Private\Programmeren\GitHub\a_simple_accounting_program\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C523224D-4711-459C-A459-990679624774}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F160D692-1BFC-42AB-A8DB-0670A356BBFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6045" yWindow="2520" windowWidth="19575" windowHeight="13080" xr2:uid="{75B15438-B83E-4BD5-B67E-78D6D5B1B1A3}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="19575" windowHeight="13080" xr2:uid="{75B15438-B83E-4BD5-B67E-78D6D5B1B1A3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Template" sheetId="1" r:id="rId1"/>
+    <sheet name="Factuur" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Template!$A$1:$H$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Factuur!$A$1:$H$36</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
-  <si>
-    <t>Denise Boezaard</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -925,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D9198C4-6966-4957-A9E3-10D25347C1DA}">
-  <dimension ref="A2:I38"/>
+  <dimension ref="A2:I37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:XFD39"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -943,37 +940,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="1"/>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="F3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="F5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="F6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -981,20 +976,20 @@
     </row>
     <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="F8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>9</v>
       </c>
       <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="F9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>11</v>
       </c>
       <c r="H9" s="9"/>
     </row>
@@ -1004,41 +999,41 @@
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="11"/>
     </row>
     <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="11"/>
     </row>
     <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="11"/>
     </row>
     <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="F16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="F17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="13" t="s">
         <v>18</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1046,49 +1041,49 @@
     </row>
     <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="14" t="s">
-        <v>21</v>
-      </c>
       <c r="G19" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="15" t="s">
         <v>22</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>23</v>
       </c>
       <c r="F20" s="16"/>
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="15" t="s">
         <v>24</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>25</v>
       </c>
       <c r="F21" s="16"/>
     </row>
     <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F23" s="18"/>
     </row>
@@ -1098,91 +1093,91 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D25" s="17"/>
     </row>
     <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="20" t="s">
         <v>31</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>32</v>
       </c>
       <c r="C26" s="21"/>
       <c r="D26" s="22"/>
       <c r="E26" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="22" t="s">
+      <c r="G26" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="G26" s="22" t="s">
+      <c r="H26" s="23" t="s">
         <v>35</v>
-      </c>
-      <c r="H26" s="23" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="25" t="s">
+      <c r="F27" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="F27" s="25" t="s">
+      <c r="G27" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="G27" s="26" t="s">
+      <c r="H27" s="27" t="s">
         <v>40</v>
-      </c>
-      <c r="H27" s="27" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="H28" s="29" t="s">
         <v>43</v>
-      </c>
-      <c r="H28" s="29" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="H29" s="30" t="s">
         <v>46</v>
-      </c>
-      <c r="H29" s="30" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="31" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B30" s="32"/>
       <c r="C30" s="32"/>
       <c r="D30" s="32"/>
       <c r="E30" s="33" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30" s="33"/>
       <c r="G30" s="33" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H30" s="34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -1195,85 +1190,75 @@
       <c r="G31" s="33"/>
       <c r="H31" s="34"/>
     </row>
-    <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="31"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="34"/>
+    <row r="32" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="36"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="36"/>
+      <c r="H32" s="37" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="33" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="37" t="s">
+      <c r="A33" s="38" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="38" t="s">
+      <c r="B33" s="39"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="41"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="B34" s="39"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="41"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B34" s="42"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="42"/>
+    </row>
+    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="42" t="s">
         <v>52</v>
       </c>
       <c r="B35" s="42"/>
-      <c r="C35" s="42"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="42"/>
-      <c r="G35" s="42"/>
-      <c r="H35" s="42"/>
-    </row>
-    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="C35" s="2"/>
+      <c r="E35" s="42" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="42" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B36" s="42"/>
-      <c r="C36" s="2"/>
-      <c r="E36" s="42" t="s">
-        <v>54</v>
-      </c>
+      <c r="C36" s="42"/>
+      <c r="E36" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="I36" s="42"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="42" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B37" s="42"/>
-      <c r="C37" s="42"/>
-      <c r="E37" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="I37" s="42"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="42" t="s">
+      <c r="C37" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" s="44" t="s">
         <v>57</v>
-      </c>
-      <c r="B38" s="42"/>
-      <c r="C38" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="E38" s="44" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
replaced terms from worksheet for invoice and some for client
</commit_message>
<xml_diff>
--- a/input_files/invoice_template.xlsx
+++ b/input_files/invoice_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Private\Programmeren\GitHub\a_simple_accounting_program\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F160D692-1BFC-42AB-A8DB-0670A356BBFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DC8401-6F25-42FF-A6B2-123DA3B88DE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="19575" windowHeight="13080" xr2:uid="{75B15438-B83E-4BD5-B67E-78D6D5B1B1A3}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="19575" windowHeight="13080" xr2:uid="{75B15438-B83E-4BD5-B67E-78D6D5B1B1A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Factuur" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -195,19 +195,10 @@
     <t>te maken op rekening</t>
   </si>
   <si>
-    <t>#link_to_my_IBAN</t>
-  </si>
-  <si>
     <t>onder vermelding van factuurnummer</t>
   </si>
   <si>
-    <t>#link_to_invoice_number</t>
-  </si>
-  <si>
     <t>en factuurdatum</t>
-  </si>
-  <si>
-    <t>#link_to_invoice_date</t>
   </si>
 </sst>
 </file>
@@ -924,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D9198C4-6966-4957-A9E3-10D25347C1DA}">
   <dimension ref="A2:I37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1234,31 +1225,34 @@
       </c>
       <c r="B35" s="42"/>
       <c r="C35" s="2"/>
-      <c r="E35" s="42" t="s">
-        <v>53</v>
+      <c r="E35" s="42" t="str">
+        <f>$G$8</f>
+        <v>My IBAN</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B36" s="42"/>
       <c r="C36" s="42"/>
-      <c r="E36" s="43" t="s">
-        <v>55</v>
+      <c r="E36" s="43" t="str">
+        <f>$H$16</f>
+        <v>#invoice_number</v>
       </c>
       <c r="I36" s="42"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="42" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B37" s="42"/>
       <c r="C37" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="E37" s="44" t="s">
-        <v>57</v>
+      <c r="E37" s="44" t="str">
+        <f>$H$17</f>
+        <v>#invoice_date</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add single working day to invoice (not multiple)
</commit_message>
<xml_diff>
--- a/input_files/invoice_template.xlsx
+++ b/input_files/invoice_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Private\Programmeren\GitHub\a_simple_accounting_program\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DC8401-6F25-42FF-A6B2-123DA3B88DE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869117C6-D70A-4C94-9534-2A87FD8B5D02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="19575" windowHeight="13080" xr2:uid="{75B15438-B83E-4BD5-B67E-78D6D5B1B1A3}"/>
+    <workbookView xWindow="2160" yWindow="2160" windowWidth="19575" windowHeight="13080" xr2:uid="{75B15438-B83E-4BD5-B67E-78D6D5B1B1A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Factuur" sheetId="1" r:id="rId1"/>
@@ -165,18 +165,12 @@
     <t>#times_commute_km</t>
   </si>
   <si>
-    <t>#calculated_amount_for_commute_km</t>
-  </si>
-  <si>
     <t>- Gereden voor de praktijk (in kilometers)</t>
   </si>
   <si>
     <t>#times_distance_during_work_km</t>
   </si>
   <si>
-    <t>#calculated_amount_for_distance_during_work_km</t>
-  </si>
-  <si>
     <t>#calculated_amount_for_working_day</t>
   </si>
   <si>
@@ -199,6 +193,12 @@
   </si>
   <si>
     <t>en factuurdatum</t>
+  </si>
+  <si>
+    <t>#calculated_amount_for_commute</t>
+  </si>
+  <si>
+    <t>#calculated_amount_for_distance_during_work</t>
   </si>
 </sst>
 </file>
@@ -916,7 +916,7 @@
   <dimension ref="A2:I37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1137,20 +1137,20 @@
         <v>42</v>
       </c>
       <c r="H28" s="29" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H29" s="30" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -1168,7 +1168,7 @@
         <v>0</v>
       </c>
       <c r="H30" s="34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -1183,7 +1183,7 @@
     </row>
     <row r="32" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="35" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B32" s="36"/>
       <c r="C32" s="36"/>
@@ -1192,12 +1192,12 @@
       <c r="F32" s="36"/>
       <c r="G32" s="36"/>
       <c r="H32" s="37" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="38" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B33" s="39"/>
       <c r="C33" s="39"/>
@@ -1209,7 +1209,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="42" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B34" s="42"/>
       <c r="C34" s="42"/>
@@ -1221,7 +1221,7 @@
     </row>
     <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="42" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B35" s="42"/>
       <c r="C35" s="2"/>
@@ -1232,7 +1232,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="42" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B36" s="42"/>
       <c r="C36" s="42"/>
@@ -1244,7 +1244,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="42" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B37" s="42"/>
       <c r="C37" s="42" t="s">

</xml_diff>

<commit_message>
added type of hours with translation; fixed calculation of total amount
</commit_message>
<xml_diff>
--- a/input_files/invoice_template.xlsx
+++ b/input_files/invoice_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Private\Programmeren\GitHub\a_simple_accounting_program\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869117C6-D70A-4C94-9534-2A87FD8B5D02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523C22B3-01E3-41F2-B775-9896796EB1FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2160" yWindow="2160" windowWidth="19575" windowHeight="13080" xr2:uid="{75B15438-B83E-4BD5-B67E-78D6D5B1B1A3}"/>
   </bookViews>
@@ -463,7 +463,7 @@
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="15"/>
@@ -529,6 +529,9 @@
     <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -915,8 +918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D9198C4-6966-4957-A9E3-10D25347C1DA}">
   <dimension ref="A2:I37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1172,14 +1175,14 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="31"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="34"/>
+      <c r="A31" s="45"/>
+      <c r="B31" s="46"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="47"/>
     </row>
     <row r="32" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="35" t="s">

</xml_diff>

<commit_message>
zipped backup to user directory, with folder structure preserved inside zipfile, no second backup location yet
</commit_message>
<xml_diff>
--- a/input_files/invoice_template.xlsx
+++ b/input_files/invoice_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Private\Programmeren\GitHub\a_simple_accounting_program\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523C22B3-01E3-41F2-B775-9896796EB1FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4C962C-E8E1-44F9-A2CE-29C046B92724}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="2160" windowWidth="19575" windowHeight="13080" xr2:uid="{75B15438-B83E-4BD5-B67E-78D6D5B1B1A3}"/>
+    <workbookView xWindow="10275" yWindow="1665" windowWidth="19575" windowHeight="13080" xr2:uid="{75B15438-B83E-4BD5-B67E-78D6D5B1B1A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Factuur" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -199,6 +199,30 @@
   </si>
   <si>
     <t>#calculated_amount_for_distance_during_work</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
   </si>
 </sst>
 </file>
@@ -919,7 +943,7 @@
   <dimension ref="A2:I37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:H31"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1175,14 +1199,30 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="45"/>
-      <c r="B31" s="46"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="47"/>
+      <c r="A31" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="G31" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="H31" s="47" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="32" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="35" t="s">

</xml_diff>